<commit_message>
Added history icon for category
</commit_message>
<xml_diff>
--- a/ComplaintManagement/Imports/Samples/Committee/Committee.xlsx
+++ b/ComplaintManagement/Imports/Samples/Committee/Committee.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Ankur\ComplaintManagement\ComplaintManagement\Imports\Samples\Committee\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\ComplaintManagement\ComplaintManagement\Imports\Samples\Committee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FA0345-32DD-4239-8487-96A3F061923B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0AA4D0E-40E3-4C37-92E2-ED18BF8F9D34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{3790FE9A-06EF-4AE6-B0AA-BD27AF2146F6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{3790FE9A-06EF-4AE6-B0AA-BD27AF2146F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Status</t>
   </si>
@@ -58,6 +58,30 @@
   </si>
   <si>
     <t>CommitteeName</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Harshita sharma</t>
+  </si>
+  <si>
+    <t>ketan Sali</t>
+  </si>
+  <si>
+    <t>Himanshu</t>
+  </si>
+  <si>
+    <t>juku</t>
+  </si>
+  <si>
+    <t>aaaaaa</t>
+  </si>
+  <si>
+    <t>Akshay Bhagwat</t>
+  </si>
+  <si>
+    <t>Manoj N</t>
   </si>
 </sst>
 </file>
@@ -409,75 +433,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D3F523-598D-402E-A543-FD1A8A3368D3}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added imports in all modules - Akshay
</commit_message>
<xml_diff>
--- a/ComplaintManagement/Imports/Samples/Committee/Committee.xlsx
+++ b/ComplaintManagement/Imports/Samples/Committee/Committee.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Ankur\ComplaintManagement\ComplaintManagement\Imports\Samples\Committee\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\India\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FA0345-32DD-4239-8487-96A3F061923B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF90D95-52A6-4B54-9902-8C0E78411B86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{3790FE9A-06EF-4AE6-B0AA-BD27AF2146F6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{3790FE9A-06EF-4AE6-B0AA-BD27AF2146F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Status</t>
   </si>
@@ -45,19 +45,19 @@
     <t>cc</t>
   </si>
   <si>
-    <t>dd</t>
-  </si>
-  <si>
-    <t>ee</t>
-  </si>
-  <si>
-    <t>ff</t>
-  </si>
-  <si>
-    <t>gg</t>
-  </si>
-  <si>
     <t>CommitteeName</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>ketan Sali,aaaaaa</t>
+  </si>
+  <si>
+    <t>Harshita sharma,Akshay Bhagwat</t>
+  </si>
+  <si>
+    <t>Himanshu,juku</t>
   </si>
 </sst>
 </file>
@@ -409,75 +409,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D3F523-598D-402E-A543-FD1A8A3368D3}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>